<commit_message>
borders fix for excel cells
</commit_message>
<xml_diff>
--- a/data/jira/OSIVnet Release Notes Template.xlsx
+++ b/data/jira/OSIVnet Release Notes Template.xlsx
@@ -163,7 +163,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -180,12 +180,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -201,6 +201,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,9 +256,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>235440</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -264,7 +272,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3255480" cy="857160"/>
+          <a:ext cx="3255120" cy="856800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -459,7 +467,7 @@
   <dimension ref="A2:F427"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -625,1489 +633,1489 @@
       <c r="F22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="9"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="9"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="9"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="9"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="9"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="9"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="9"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="9"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="9"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="9"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="9"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="9"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="9"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="9"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="9"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="9"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="9"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="9"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="9"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="9"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="9"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="9"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="9"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="9"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="9"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="11"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="9"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="9"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="9"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="9"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="11"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="9"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="11"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="9"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="11"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="9"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="11"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="9"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="11"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="9"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="11"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="9"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="11"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="9"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="11"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="9"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="11"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="9"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="11"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="9"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="11"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="9"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="11"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="9"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="11"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="9"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="11"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="9"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="11"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="9"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="11"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="9"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="9"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="11"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="9"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="11"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="9"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="11"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="9"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="11"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="9"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="11"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="9"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="11"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F77" s="10"/>
+      <c r="F77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F78" s="10"/>
+      <c r="F78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F79" s="10"/>
+      <c r="F79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F80" s="10"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F81" s="10"/>
+      <c r="F81" s="12"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F82" s="10"/>
+      <c r="F82" s="12"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F83" s="10"/>
+      <c r="F83" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F84" s="10"/>
+      <c r="F84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F85" s="10"/>
+      <c r="F85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F86" s="10"/>
+      <c r="F86" s="12"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F87" s="10"/>
+      <c r="F87" s="12"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F88" s="10"/>
+      <c r="F88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F89" s="10"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F90" s="10"/>
+      <c r="F90" s="12"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F91" s="10"/>
+      <c r="F91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F92" s="10"/>
+      <c r="F92" s="12"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F93" s="10"/>
+      <c r="F93" s="12"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F94" s="10"/>
+      <c r="F94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F95" s="10"/>
+      <c r="F95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F96" s="10"/>
+      <c r="F96" s="12"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F97" s="10"/>
+      <c r="F97" s="12"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F98" s="10"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F99" s="10"/>
+      <c r="F99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F100" s="10"/>
+      <c r="F100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F101" s="10"/>
+      <c r="F101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F102" s="10"/>
+      <c r="F102" s="12"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F103" s="10"/>
+      <c r="F103" s="12"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F104" s="10"/>
+      <c r="F104" s="12"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F105" s="10"/>
+      <c r="F105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F106" s="10"/>
+      <c r="F106" s="12"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F107" s="10"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F108" s="10"/>
+      <c r="F108" s="12"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F109" s="10"/>
+      <c r="F109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F110" s="10"/>
+      <c r="F110" s="12"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F111" s="10"/>
+      <c r="F111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F112" s="10"/>
+      <c r="F112" s="12"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F113" s="10"/>
+      <c r="F113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F114" s="10"/>
+      <c r="F114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F115" s="10"/>
+      <c r="F115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F116" s="10"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F117" s="10"/>
+      <c r="F117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F118" s="10"/>
+      <c r="F118" s="12"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F119" s="10"/>
+      <c r="F119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F120" s="10"/>
+      <c r="F120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F121" s="10"/>
+      <c r="F121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F122" s="10"/>
+      <c r="F122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F123" s="10"/>
+      <c r="F123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F124" s="10"/>
+      <c r="F124" s="12"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F125" s="10"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F126" s="10"/>
+      <c r="F126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F127" s="10"/>
+      <c r="F127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F128" s="10"/>
+      <c r="F128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F129" s="10"/>
+      <c r="F129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F130" s="10"/>
+      <c r="F130" s="12"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F131" s="10"/>
+      <c r="F131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F132" s="10"/>
+      <c r="F132" s="12"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F133" s="10"/>
+      <c r="F133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F134" s="10"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F135" s="10"/>
+      <c r="F135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F136" s="10"/>
+      <c r="F136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F137" s="10"/>
+      <c r="F137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F138" s="10"/>
+      <c r="F138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F139" s="10"/>
+      <c r="F139" s="12"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F140" s="10"/>
+      <c r="F140" s="12"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F141" s="10"/>
+      <c r="F141" s="12"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F142" s="10"/>
+      <c r="F142" s="12"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F143" s="10"/>
+      <c r="F143" s="12"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F144" s="10"/>
+      <c r="F144" s="12"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F145" s="10"/>
+      <c r="F145" s="12"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F146" s="10"/>
+      <c r="F146" s="12"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F147" s="10"/>
+      <c r="F147" s="12"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F148" s="10"/>
+      <c r="F148" s="12"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F149" s="10"/>
+      <c r="F149" s="12"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F150" s="10"/>
+      <c r="F150" s="12"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F151" s="10"/>
+      <c r="F151" s="12"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F152" s="10"/>
+      <c r="F152" s="12"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F153" s="10"/>
+      <c r="F153" s="12"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F154" s="10"/>
+      <c r="F154" s="12"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F155" s="10"/>
+      <c r="F155" s="12"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F156" s="10"/>
+      <c r="F156" s="12"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F157" s="10"/>
+      <c r="F157" s="12"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F158" s="10"/>
+      <c r="F158" s="12"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F159" s="10"/>
+      <c r="F159" s="12"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F160" s="10"/>
+      <c r="F160" s="12"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F161" s="10"/>
+      <c r="F161" s="12"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F162" s="10"/>
+      <c r="F162" s="12"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F163" s="10"/>
+      <c r="F163" s="12"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F164" s="10"/>
+      <c r="F164" s="12"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F165" s="10"/>
+      <c r="F165" s="12"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F166" s="10"/>
+      <c r="F166" s="12"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F167" s="10"/>
+      <c r="F167" s="12"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F168" s="10"/>
+      <c r="F168" s="12"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F169" s="10"/>
+      <c r="F169" s="12"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F170" s="10"/>
+      <c r="F170" s="12"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F171" s="10"/>
+      <c r="F171" s="12"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F172" s="10"/>
+      <c r="F172" s="12"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F173" s="10"/>
+      <c r="F173" s="12"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F174" s="10"/>
+      <c r="F174" s="12"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F175" s="10"/>
+      <c r="F175" s="12"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F176" s="10"/>
+      <c r="F176" s="12"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F177" s="10"/>
+      <c r="F177" s="12"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F178" s="10"/>
+      <c r="F178" s="12"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F179" s="10"/>
+      <c r="F179" s="12"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F180" s="10"/>
+      <c r="F180" s="12"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F181" s="10"/>
+      <c r="F181" s="12"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F182" s="10"/>
+      <c r="F182" s="12"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F183" s="10"/>
+      <c r="F183" s="12"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F184" s="10"/>
+      <c r="F184" s="12"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F185" s="10"/>
+      <c r="F185" s="12"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F186" s="10"/>
+      <c r="F186" s="12"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F187" s="10"/>
+      <c r="F187" s="12"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F188" s="10"/>
+      <c r="F188" s="12"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F189" s="10"/>
+      <c r="F189" s="12"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F190" s="10"/>
+      <c r="F190" s="12"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F191" s="10"/>
+      <c r="F191" s="12"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F192" s="10"/>
+      <c r="F192" s="12"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F193" s="10"/>
+      <c r="F193" s="12"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F194" s="10"/>
+      <c r="F194" s="12"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F195" s="10"/>
+      <c r="F195" s="12"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F196" s="10"/>
+      <c r="F196" s="12"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F197" s="10"/>
+      <c r="F197" s="12"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F198" s="10"/>
+      <c r="F198" s="12"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F199" s="10"/>
+      <c r="F199" s="12"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F200" s="10"/>
+      <c r="F200" s="12"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F201" s="10"/>
+      <c r="F201" s="12"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F202" s="10"/>
+      <c r="F202" s="12"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F203" s="10"/>
+      <c r="F203" s="12"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F204" s="10"/>
+      <c r="F204" s="12"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F205" s="10"/>
+      <c r="F205" s="12"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F206" s="10"/>
+      <c r="F206" s="12"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F207" s="10"/>
+      <c r="F207" s="12"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F208" s="10"/>
+      <c r="F208" s="12"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F209" s="10"/>
+      <c r="F209" s="12"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F210" s="10"/>
+      <c r="F210" s="12"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F211" s="10"/>
+      <c r="F211" s="12"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F212" s="10"/>
+      <c r="F212" s="12"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F213" s="10"/>
+      <c r="F213" s="12"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F214" s="10"/>
+      <c r="F214" s="12"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F215" s="10"/>
+      <c r="F215" s="12"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F216" s="10"/>
+      <c r="F216" s="12"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F217" s="10"/>
+      <c r="F217" s="12"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F218" s="10"/>
+      <c r="F218" s="12"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F219" s="10"/>
+      <c r="F219" s="12"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F220" s="10"/>
+      <c r="F220" s="12"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F221" s="10"/>
+      <c r="F221" s="12"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F222" s="10"/>
+      <c r="F222" s="12"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F223" s="10"/>
+      <c r="F223" s="12"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F224" s="10"/>
+      <c r="F224" s="12"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F225" s="10"/>
+      <c r="F225" s="12"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F226" s="10"/>
+      <c r="F226" s="12"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F227" s="10"/>
+      <c r="F227" s="12"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F228" s="10"/>
+      <c r="F228" s="12"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F229" s="10"/>
+      <c r="F229" s="12"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F230" s="10"/>
+      <c r="F230" s="12"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F231" s="10"/>
+      <c r="F231" s="12"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F232" s="10"/>
+      <c r="F232" s="12"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F233" s="10"/>
+      <c r="F233" s="12"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F234" s="10"/>
+      <c r="F234" s="12"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F235" s="10"/>
+      <c r="F235" s="12"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F236" s="10"/>
+      <c r="F236" s="12"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F237" s="10"/>
+      <c r="F237" s="12"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F238" s="10"/>
+      <c r="F238" s="12"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F239" s="10"/>
+      <c r="F239" s="12"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F240" s="10"/>
+      <c r="F240" s="12"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F241" s="10"/>
+      <c r="F241" s="12"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F242" s="10"/>
+      <c r="F242" s="12"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F243" s="10"/>
+      <c r="F243" s="12"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F244" s="10"/>
+      <c r="F244" s="12"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F245" s="10"/>
+      <c r="F245" s="12"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F246" s="10"/>
+      <c r="F246" s="12"/>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F247" s="10"/>
+      <c r="F247" s="12"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F248" s="10"/>
+      <c r="F248" s="12"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F249" s="10"/>
+      <c r="F249" s="12"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F250" s="10"/>
+      <c r="F250" s="12"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F251" s="10"/>
+      <c r="F251" s="12"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F252" s="10"/>
+      <c r="F252" s="12"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F253" s="10"/>
+      <c r="F253" s="12"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F254" s="10"/>
+      <c r="F254" s="12"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F255" s="10"/>
+      <c r="F255" s="12"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F256" s="10"/>
+      <c r="F256" s="12"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F257" s="10"/>
+      <c r="F257" s="12"/>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F258" s="10"/>
+      <c r="F258" s="12"/>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F259" s="10"/>
+      <c r="F259" s="12"/>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F260" s="10"/>
+      <c r="F260" s="12"/>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F261" s="10"/>
+      <c r="F261" s="12"/>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F262" s="10"/>
+      <c r="F262" s="12"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F263" s="10"/>
+      <c r="F263" s="12"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F264" s="10"/>
+      <c r="F264" s="12"/>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F265" s="10"/>
+      <c r="F265" s="12"/>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F266" s="10"/>
+      <c r="F266" s="12"/>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F267" s="10"/>
+      <c r="F267" s="12"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F268" s="10"/>
+      <c r="F268" s="12"/>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F269" s="10"/>
+      <c r="F269" s="12"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F270" s="10"/>
+      <c r="F270" s="12"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F271" s="10"/>
+      <c r="F271" s="12"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F272" s="10"/>
+      <c r="F272" s="12"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F273" s="10"/>
+      <c r="F273" s="12"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F274" s="10"/>
+      <c r="F274" s="12"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F275" s="10"/>
+      <c r="F275" s="12"/>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F276" s="10"/>
+      <c r="F276" s="12"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F277" s="10"/>
+      <c r="F277" s="12"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F278" s="10"/>
+      <c r="F278" s="12"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F279" s="10"/>
+      <c r="F279" s="12"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F280" s="10"/>
+      <c r="F280" s="12"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F281" s="10"/>
+      <c r="F281" s="12"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F282" s="10"/>
+      <c r="F282" s="12"/>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F283" s="10"/>
+      <c r="F283" s="12"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F284" s="10"/>
+      <c r="F284" s="12"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F285" s="10"/>
+      <c r="F285" s="12"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F286" s="10"/>
+      <c r="F286" s="12"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F287" s="10"/>
+      <c r="F287" s="12"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F288" s="10"/>
+      <c r="F288" s="12"/>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F289" s="10"/>
+      <c r="F289" s="12"/>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F290" s="10"/>
+      <c r="F290" s="12"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F291" s="10"/>
+      <c r="F291" s="12"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F292" s="10"/>
+      <c r="F292" s="12"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F293" s="10"/>
+      <c r="F293" s="12"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F294" s="10"/>
+      <c r="F294" s="12"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F295" s="10"/>
+      <c r="F295" s="12"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F296" s="10"/>
+      <c r="F296" s="12"/>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F297" s="10"/>
+      <c r="F297" s="12"/>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F298" s="10"/>
+      <c r="F298" s="12"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F299" s="10"/>
+      <c r="F299" s="12"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F300" s="10"/>
+      <c r="F300" s="12"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F301" s="10"/>
+      <c r="F301" s="12"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F302" s="10"/>
+      <c r="F302" s="12"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F303" s="10"/>
+      <c r="F303" s="12"/>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F304" s="10"/>
+      <c r="F304" s="12"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F305" s="10"/>
+      <c r="F305" s="12"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F306" s="10"/>
+      <c r="F306" s="12"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F307" s="10"/>
+      <c r="F307" s="12"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F308" s="10"/>
+      <c r="F308" s="12"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F309" s="10"/>
+      <c r="F309" s="12"/>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F310" s="10"/>
+      <c r="F310" s="12"/>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F311" s="10"/>
+      <c r="F311" s="12"/>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F312" s="10"/>
+      <c r="F312" s="12"/>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F313" s="10"/>
+      <c r="F313" s="12"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F314" s="10"/>
+      <c r="F314" s="12"/>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F315" s="10"/>
+      <c r="F315" s="12"/>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F316" s="10"/>
+      <c r="F316" s="12"/>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F317" s="10"/>
+      <c r="F317" s="12"/>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F318" s="10"/>
+      <c r="F318" s="12"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F319" s="10"/>
+      <c r="F319" s="12"/>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F320" s="10"/>
+      <c r="F320" s="12"/>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F321" s="10"/>
+      <c r="F321" s="12"/>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F322" s="10"/>
+      <c r="F322" s="12"/>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F323" s="10"/>
+      <c r="F323" s="12"/>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F324" s="10"/>
+      <c r="F324" s="12"/>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F325" s="10"/>
+      <c r="F325" s="12"/>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F326" s="10"/>
+      <c r="F326" s="12"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F327" s="10"/>
+      <c r="F327" s="12"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F328" s="10"/>
+      <c r="F328" s="12"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F329" s="10"/>
+      <c r="F329" s="12"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F330" s="10"/>
+      <c r="F330" s="12"/>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F331" s="10"/>
+      <c r="F331" s="12"/>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F332" s="10"/>
+      <c r="F332" s="12"/>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F333" s="10"/>
+      <c r="F333" s="12"/>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F334" s="10"/>
+      <c r="F334" s="12"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F335" s="10"/>
+      <c r="F335" s="12"/>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F336" s="10"/>
+      <c r="F336" s="12"/>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F337" s="10"/>
+      <c r="F337" s="12"/>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F338" s="10"/>
+      <c r="F338" s="12"/>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F339" s="10"/>
+      <c r="F339" s="12"/>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F340" s="10"/>
+      <c r="F340" s="12"/>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F341" s="10"/>
+      <c r="F341" s="12"/>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F342" s="10"/>
+      <c r="F342" s="12"/>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F343" s="10"/>
+      <c r="F343" s="12"/>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F344" s="10"/>
+      <c r="F344" s="12"/>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F345" s="10"/>
+      <c r="F345" s="12"/>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F346" s="10"/>
+      <c r="F346" s="12"/>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F347" s="10"/>
+      <c r="F347" s="12"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F348" s="10"/>
+      <c r="F348" s="12"/>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F349" s="10"/>
+      <c r="F349" s="12"/>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F350" s="10"/>
+      <c r="F350" s="12"/>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F351" s="10"/>
+      <c r="F351" s="12"/>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F352" s="10"/>
+      <c r="F352" s="12"/>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F353" s="10"/>
+      <c r="F353" s="12"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F354" s="10"/>
+      <c r="F354" s="12"/>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F355" s="10"/>
+      <c r="F355" s="12"/>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F356" s="10"/>
+      <c r="F356" s="12"/>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F357" s="10"/>
+      <c r="F357" s="12"/>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F358" s="10"/>
+      <c r="F358" s="12"/>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F359" s="10"/>
+      <c r="F359" s="12"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F360" s="10"/>
+      <c r="F360" s="12"/>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F361" s="10"/>
+      <c r="F361" s="12"/>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F362" s="10"/>
+      <c r="F362" s="12"/>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F363" s="10"/>
+      <c r="F363" s="12"/>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F364" s="10"/>
+      <c r="F364" s="12"/>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F365" s="10"/>
+      <c r="F365" s="12"/>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F366" s="10"/>
+      <c r="F366" s="12"/>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F367" s="10"/>
+      <c r="F367" s="12"/>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F368" s="10"/>
+      <c r="F368" s="12"/>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F369" s="10"/>
+      <c r="F369" s="12"/>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F370" s="10"/>
+      <c r="F370" s="12"/>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F371" s="10"/>
+      <c r="F371" s="12"/>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F372" s="10"/>
+      <c r="F372" s="12"/>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F373" s="10"/>
+      <c r="F373" s="12"/>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F374" s="10"/>
+      <c r="F374" s="12"/>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F375" s="10"/>
+      <c r="F375" s="12"/>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F376" s="10"/>
+      <c r="F376" s="12"/>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F377" s="10"/>
+      <c r="F377" s="12"/>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F378" s="10"/>
+      <c r="F378" s="12"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F379" s="10"/>
+      <c r="F379" s="12"/>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F380" s="10"/>
+      <c r="F380" s="12"/>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F381" s="10"/>
+      <c r="F381" s="12"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F382" s="10"/>
+      <c r="F382" s="12"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F383" s="10"/>
+      <c r="F383" s="12"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F384" s="10"/>
+      <c r="F384" s="12"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F385" s="10"/>
+      <c r="F385" s="12"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F386" s="10"/>
+      <c r="F386" s="12"/>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F387" s="10"/>
+      <c r="F387" s="12"/>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F388" s="10"/>
+      <c r="F388" s="12"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F389" s="10"/>
+      <c r="F389" s="12"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F390" s="10"/>
+      <c r="F390" s="12"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F391" s="10"/>
+      <c r="F391" s="12"/>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F392" s="10"/>
+      <c r="F392" s="12"/>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F393" s="10"/>
+      <c r="F393" s="12"/>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F394" s="10"/>
+      <c r="F394" s="12"/>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F395" s="10"/>
+      <c r="F395" s="12"/>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F396" s="10"/>
+      <c r="F396" s="12"/>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F397" s="10"/>
+      <c r="F397" s="12"/>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F398" s="10"/>
+      <c r="F398" s="12"/>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F399" s="10"/>
+      <c r="F399" s="12"/>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F400" s="10"/>
+      <c r="F400" s="12"/>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F401" s="10"/>
+      <c r="F401" s="12"/>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F402" s="10"/>
+      <c r="F402" s="12"/>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F403" s="10"/>
+      <c r="F403" s="12"/>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F404" s="10"/>
+      <c r="F404" s="12"/>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F405" s="10"/>
+      <c r="F405" s="12"/>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F406" s="10"/>
+      <c r="F406" s="12"/>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F407" s="10"/>
+      <c r="F407" s="12"/>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F408" s="10"/>
+      <c r="F408" s="12"/>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F409" s="10"/>
+      <c r="F409" s="12"/>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F410" s="10"/>
+      <c r="F410" s="12"/>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F411" s="10"/>
+      <c r="F411" s="12"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F412" s="10"/>
+      <c r="F412" s="12"/>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F413" s="10"/>
+      <c r="F413" s="12"/>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F414" s="10"/>
+      <c r="F414" s="12"/>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F415" s="10"/>
+      <c r="F415" s="12"/>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F416" s="10"/>
+      <c r="F416" s="12"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F417" s="10"/>
+      <c r="F417" s="12"/>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F418" s="10"/>
+      <c r="F418" s="12"/>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F419" s="10"/>
+      <c r="F419" s="12"/>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F420" s="10"/>
+      <c r="F420" s="12"/>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F421" s="10"/>
+      <c r="F421" s="12"/>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F422" s="10"/>
+      <c r="F422" s="12"/>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F423" s="10"/>
+      <c r="F423" s="12"/>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F424" s="10"/>
+      <c r="F424" s="12"/>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F425" s="10"/>
+      <c r="F425" s="12"/>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F426" s="10"/>
+      <c r="F426" s="12"/>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F427" s="10"/>
+      <c r="F427" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:F8"/>

</xml_diff>